<commit_message>
external media zip import
</commit_message>
<xml_diff>
--- a/app_kit/tests/TESTS_ROOT/xlsx_for_testing/TaxonProfiles/valid/Taxon profiles.xlsx
+++ b/app_kit/tests/TESTS_ROOT/xlsx_for_testing/TaxonProfiles/valid/Taxon profiles.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Taxon Profiles" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Taxon Profile Images" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="External Media" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="84">
   <si>
     <t xml:space="preserve">Scientific Name</t>
   </si>
@@ -56,6 +57,9 @@
     <t xml:space="preserve">tags</t>
   </si>
   <si>
+    <t xml:space="preserve">external_media</t>
+  </si>
+  <si>
     <t xml:space="preserve">Interesting facts</t>
   </si>
   <si>
@@ -80,6 +84,24 @@
     <t xml:space="preserve">meta_description</t>
   </si>
   <si>
+    <t xml:space="preserve">youtube</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wav</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test category</t>
   </si>
   <si>
@@ -131,6 +153,27 @@
     <t xml:space="preserve">tree, deciduous</t>
   </si>
   <si>
+    <t xml:space="preserve">https://code-for-nature.com/images/Biodiversity-illustration-screen-sm.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=v5ekOVJ5uzU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://samplelib.com/lib/preview/mp3/sample-3s.mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://samplelib.com/lib/preview/wav/sample-3s.wav</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://file-examples.com/storage/fe42043ddc68bdea5933232/2017/10/file-sample_150kB.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://code-for-nature.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://file-examples.com/wp-content/storage/2017/02/file_example_CSV_5000.csv</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fraxinus excelsior</t>
   </si>
   <si>
@@ -186,6 +229,51 @@
   </si>
   <si>
     <t xml:space="preserve">Leaf alt text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licence (optional)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biodiversity illustration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">external media author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">external media licence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">external media caption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">external media alt text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patchwork Cuttlefish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample mp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample wav</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample file</t>
   </si>
 </sst>
 </file>
@@ -196,7 +284,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -221,6 +309,13 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -287,7 +382,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -313,6 +408,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="fill" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -324,12 +423,16 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="fill" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -541,8 +644,8 @@
   </sheetPr>
   <dimension ref="A1:AMP27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J31" activeCellId="0" sqref="J31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X4" activeCellId="0" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -556,6 +659,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="23.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="33.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="19.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="62.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="48.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="47.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="46.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="63.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="24.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="2" width="24.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -602,13 +712,27 @@
       <c r="Q1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
+      <c r="R1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
       <c r="AA1" s="5"/>
@@ -1623,44 +1747,58 @@
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="M2" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
+      <c r="R2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
@@ -2679,16 +2817,16 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -3709,295 +3847,329 @@
       <c r="AMP3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="6" t="s">
+      <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="F4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="J4" s="7" t="s">
         <v>35</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="U4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="V4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="W4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="X4" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="191.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
+      <c r="A5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="112.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:M5"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="U4" r:id="rId1" display="https://samplelib.com/lib/preview/wav/sample-3s.wav"/>
+    <hyperlink ref="W4" r:id="rId2" display="https://code-for-nature.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4016,14 +4188,14 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="29.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="31.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="31.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="15" width="31.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="42.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="31.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="34.51"/>
@@ -4033,58 +4205,59 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>42</v>
+        <v>55</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>56</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>54</v>
-      </c>
+      <c r="A2" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4095,4 +4268,177 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="78.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="24.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="24.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="22.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="22.95"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" display="https://samplelib.com/lib/preview/wav/sample-3s.wav"/>
+    <hyperlink ref="A7" r:id="rId2" display="https://code-for-nature.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
taxonomic relationships, bugfixes and more
</commit_message>
<xml_diff>
--- a/app_kit/tests/TESTS_ROOT/xlsx_for_testing/TaxonProfiles/valid/Taxon profiles.xlsx
+++ b/app_kit/tests/TESTS_ROOT/xlsx_for_testing/TaxonProfiles/valid/Taxon profiles.xlsx
@@ -644,8 +644,8 @@
   </sheetPr>
   <dimension ref="A1:AMP27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X4" activeCellId="0" sqref="X4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4278,7 +4278,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
taxon relationships, morphotypes, polytomous steps
</commit_message>
<xml_diff>
--- a/app_kit/tests/TESTS_ROOT/xlsx_for_testing/TaxonProfiles/valid/Taxon profiles.xlsx
+++ b/app_kit/tests/TESTS_ROOT/xlsx_for_testing/TaxonProfiles/valid/Taxon profiles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Taxon Profiles" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="87">
   <si>
     <t xml:space="preserve">Scientific Name</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t xml:space="preserve">Fraxinus excelsior occurrence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraxinus excelsior morphotype leaf short profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraxinus excelsior morphotype leaf Interesting facts</t>
   </si>
   <si>
     <t xml:space="preserve">Identifier</t>
@@ -644,8 +653,8 @@
   </sheetPr>
   <dimension ref="A1:AMP27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3940,7 +3949,21 @@
       <c r="M5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F6" s="7"/>
+      <c r="A6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>55</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -4162,10 +4185,6 @@
       <c r="M27" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:M5"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="U4" r:id="rId1" display="https://samplelib.com/lib/preview/wav/sample-3s.wav"/>
     <hyperlink ref="W4" r:id="rId2" display="https://code-for-nature.com"/>
@@ -4205,31 +4224,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4237,25 +4256,25 @@
         <v>39</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I2" s="10"/>
     </row>
@@ -4277,7 +4296,7 @@
   </sheetPr>
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4294,25 +4313,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4323,19 +4342,19 @@
         <v>8</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4346,7 +4365,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -4361,7 +4380,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -4376,7 +4395,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -4391,7 +4410,7 @@
         <v>23</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -4406,7 +4425,7 @@
         <v>24</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -4421,7 +4440,7 @@
         <v>25</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>

</xml_diff>